<commit_message>
Changed to 4 voltage scales.
Changed design from 3-scale to 4-scale. Selected a few more parts and added them to the schematic.
</commit_message>
<xml_diff>
--- a/hw/bom.xlsx
+++ b/hw/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mark\Projects\voltmeter_shield\hw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{593E7035-AF41-4A2B-BB66-82D7E9B2AC24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3994D212-E07C-43E9-B12B-347A3DF29006}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{D82A725B-82B8-4CD2-8B23-0F51E9397204}"/>
+    <workbookView xWindow="5970" yWindow="1605" windowWidth="21600" windowHeight="11385" xr2:uid="{D82A725B-82B8-4CD2-8B23-0F51E9397204}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Terminal Block</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>REFERENCE VOLTAGE</t>
+  </si>
+  <si>
+    <t>Microchip</t>
   </si>
 </sst>
 </file>
@@ -429,15 +435,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2139905-6BD5-4D6B-8ADF-B2E6ED108647}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -501,6 +507,17 @@
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -513,6 +530,7 @@
     <hyperlink ref="A6" r:id="rId6" xr:uid="{B449A9A4-CFE1-4A8C-8106-01435FE2AF22}"/>
     <hyperlink ref="A3" r:id="rId7" xr:uid="{3FA68FC5-9943-4E3C-8B46-40D1935BF0F6}"/>
     <hyperlink ref="A2" r:id="rId8" xr:uid="{A7240F6F-5FDA-4FBD-97DB-3AAC70BEB75A}"/>
+    <hyperlink ref="A11" r:id="rId9" xr:uid="{BC017FA4-0364-4453-8AEC-C583448AACAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>